<commit_message>
output updates for allocation and transitions rule with newest airtoxics nata data
</commit_message>
<xml_diff>
--- a/output/Allocation Rule/facility_data/allocation_rule_facility_demographics_10mi.xlsx
+++ b/output/Allocation Rule/facility_data/allocation_rule_facility_demographics_10mi.xlsx
@@ -32,7 +32,7 @@
     <t xml:space="preserve">pop</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_sq_mile_1mi</t>
+    <t xml:space="preserve">pop_sq_mile_10mi</t>
   </si>
   <si>
     <t xml:space="preserve">rural_facility</t>
@@ -572,10 +572,10 @@
         <v>11.8536876343167</v>
       </c>
       <c r="R2" t="n">
-        <v>36.2121212121212</v>
+        <v>37.4242424242424</v>
       </c>
       <c r="S2" t="n">
-        <v>0.454545454545455</v>
+        <v>0.440909090909091</v>
       </c>
     </row>
     <row r="3">
@@ -631,10 +631,10 @@
         <v>13.0819257713673</v>
       </c>
       <c r="R3" t="n">
-        <v>49.1891891891892</v>
+        <v>52.972972972973</v>
       </c>
       <c r="S3" t="n">
-        <v>0.537837837837838</v>
+        <v>0.510810810810811</v>
       </c>
     </row>
     <row r="4">
@@ -690,10 +690,10 @@
         <v>7.50338941192498</v>
       </c>
       <c r="R4" t="n">
-        <v>32.2368421052632</v>
+        <v>29.9013157894737</v>
       </c>
       <c r="S4" t="n">
-        <v>0.347039473684211</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="5">
@@ -749,10 +749,10 @@
         <v>5.87057212005925</v>
       </c>
       <c r="R5" t="n">
-        <v>31.4285714285714</v>
+        <v>27.1428571428571</v>
       </c>
       <c r="S5" t="n">
-        <v>0.832142857142857</v>
+        <v>0.314285714285714</v>
       </c>
     </row>
     <row r="6">
@@ -808,10 +808,10 @@
         <v>10.5272202506423</v>
       </c>
       <c r="R6" t="n">
-        <v>30.1304347826087</v>
+        <v>30.2826086956522</v>
       </c>
       <c r="S6" t="n">
-        <v>0.414782608695652</v>
+        <v>0.370217391304348</v>
       </c>
     </row>
     <row r="7">
@@ -865,10 +865,10 @@
         <v>9.70246182079913</v>
       </c>
       <c r="R7" t="n">
-        <v>29.636803874092</v>
+        <v>29.2978208232446</v>
       </c>
       <c r="S7" t="n">
-        <v>0.387409200968523</v>
+        <v>0.362953995157385</v>
       </c>
     </row>
     <row r="8">
@@ -924,10 +924,10 @@
         <v>6.6311776732443</v>
       </c>
       <c r="R8" t="n">
-        <v>79.4202898550725</v>
+        <v>53.9130434782609</v>
       </c>
       <c r="S8" t="n">
-        <v>0.521739130434783</v>
+        <v>0.427536231884058</v>
       </c>
     </row>
     <row r="9">
@@ -983,10 +983,10 @@
         <v>7.25449505337132</v>
       </c>
       <c r="R9" t="n">
-        <v>80.5882352941177</v>
+        <v>53.8235294117647</v>
       </c>
       <c r="S9" t="n">
-        <v>0.557352941176471</v>
+        <v>0.463235294117647</v>
       </c>
     </row>
     <row r="10">
@@ -1040,10 +1040,10 @@
         <v>9.26747240535932</v>
       </c>
       <c r="R10" t="n">
-        <v>20.1428571428571</v>
+        <v>20</v>
       </c>
       <c r="S10" t="n">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="11">
@@ -1099,10 +1099,10 @@
         <v>5.93507974024599</v>
       </c>
       <c r="R11" t="n">
-        <v>20</v>
+        <v>18.7878787878788</v>
       </c>
       <c r="S11" t="n">
-        <v>0.212121212121212</v>
+        <v>0.181818181818182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>